<commit_message>
cause list picture change
</commit_message>
<xml_diff>
--- a/myCBD/myInfo/gbd.ICD.MapIMAGE.xlsx
+++ b/myCBD/myInfo/gbd.ICD.MapIMAGE.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\0.CBD\myCBD\myInfo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="10935" activeTab="2"/>
   </bookViews>
@@ -20,7 +15,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$A$1:$AA$220</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -37,7 +32,7 @@
     <author>Dauphine, David (CDPH-CHSI)</author>
   </authors>
   <commentList>
-    <comment ref="Q1" authorId="0" shapeId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C57" authorId="1" shapeId="0">
+    <comment ref="C57" authorId="1">
       <text>
         <r>
           <rPr>
@@ -85,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S126" authorId="2" shapeId="0">
+    <comment ref="S126" authorId="2">
       <text>
         <r>
           <rPr>
@@ -5160,7 +5155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="###0.;###0."/>
   </numFmts>
@@ -6087,50 +6082,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -6186,7 +6138,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6221,7 +6173,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -20609,7 +20561,7 @@
         <v>1601</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="29.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="27.75" x14ac:dyDescent="0.2">
       <c r="A5" s="124" t="s">
         <v>952</v>
       </c>
@@ -24477,1062 +24429,1187 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:E122"/>
+  <dimension ref="B1:G122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E116" sqref="E116"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="124" customWidth="1"/>
     <col min="2" max="2" width="76.28515625" style="124" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.5703125" style="124" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="124"/>
-    <col min="5" max="5" width="70.140625" style="124" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="124"/>
+    <col min="3" max="4" width="2.5703125" style="124" customWidth="1"/>
+    <col min="5" max="5" width="51.5703125" style="124" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="124"/>
+    <col min="7" max="7" width="70.140625" style="124" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="124"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B2" s="154" t="s">
+    <row r="1" spans="2:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="154" t="s">
         <v>1599</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B3" s="128" t="s">
+    <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E3" s="128" t="s">
         <v>1600</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="129" t="s">
+    <row r="4" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="129" t="s">
         <v>1601</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>952</v>
       </c>
       <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B6" s="153" t="s">
         <v>1595</v>
       </c>
       <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
       <c r="E6" s="141" t="s">
+        <v>1592</v>
+      </c>
+      <c r="G6" s="141" t="s">
         <v>1593</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="155"/>
       <c r="C7" s="1"/>
-      <c r="E7" s="138" t="s">
+      <c r="D7" s="1"/>
+      <c r="E7" s="147" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="138" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B8" s="134" t="s">
         <v>1594</v>
       </c>
       <c r="C8" s="79"/>
-      <c r="E8" s="135" t="s">
+      <c r="E8" s="144" t="s">
+        <v>698</v>
+      </c>
+      <c r="F8" s="127"/>
+      <c r="G8" s="135" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="151" t="s">
         <v>1129</v>
       </c>
       <c r="C9" s="79"/>
-      <c r="E9" s="135" t="s">
+      <c r="E9" s="144" t="s">
+        <v>699</v>
+      </c>
+      <c r="F9" s="117"/>
+      <c r="G9" s="135" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="142" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="113"/>
-      <c r="E10" s="137" t="s">
+      <c r="E10" s="144" t="s">
+        <v>700</v>
+      </c>
+      <c r="F10" s="118"/>
+      <c r="G10" s="137" t="s">
         <v>717</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="139" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="114"/>
-      <c r="E11" s="137" t="s">
+      <c r="E11" s="147" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="115"/>
+      <c r="G11" s="137" t="s">
         <v>718</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="139" t="s">
         <v>1125</v>
       </c>
       <c r="C12" s="114"/>
-      <c r="E12" s="137" t="s">
+      <c r="E12" s="147" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="115"/>
+      <c r="G12" s="137" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="136" t="s">
         <v>1134</v>
       </c>
       <c r="C13" s="114"/>
-      <c r="E13" s="137" t="s">
+      <c r="E13" s="147" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="115"/>
+      <c r="G13" s="137" t="s">
         <v>720</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="144" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="115"/>
-      <c r="E14" s="142" t="s">
+      <c r="E14" s="147" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="118"/>
+      <c r="G14" s="142" t="s">
         <v>721</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="144" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="115"/>
-      <c r="E15" s="135" t="s">
+      <c r="E15" s="147" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="118"/>
+      <c r="G15" s="135" t="s">
         <v>1132</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="144" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="115"/>
-      <c r="E16" s="143" t="s">
+      <c r="E16" s="147" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="118"/>
+      <c r="G16" s="143" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="144" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="115"/>
-      <c r="E17" s="144" t="s">
+      <c r="E17" s="147" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="118"/>
+      <c r="G17" s="144" t="s">
         <v>723</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="144" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="115"/>
       <c r="E18" s="144" t="s">
+        <v>701</v>
+      </c>
+      <c r="F18" s="118"/>
+      <c r="G18" s="144" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="136" t="s">
         <v>1135</v>
       </c>
       <c r="C19" s="114"/>
-      <c r="E19" s="143" t="s">
+      <c r="E19" s="144" t="s">
+        <v>702</v>
+      </c>
+      <c r="F19" s="118"/>
+      <c r="G19" s="143" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="144" t="s">
         <v>686</v>
       </c>
       <c r="C20" s="115"/>
-      <c r="E20" s="143" t="s">
+      <c r="E20" s="139" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="118"/>
+      <c r="G20" s="143" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="144" t="s">
         <v>687</v>
       </c>
       <c r="C21" s="115"/>
-      <c r="E21" s="143" t="s">
+      <c r="E21" s="139" t="s">
+        <v>1373</v>
+      </c>
+      <c r="F21" s="115"/>
+      <c r="G21" s="143" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="137" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="114"/>
-      <c r="E22" s="143" t="s">
+      <c r="E22" s="137" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="115"/>
+      <c r="G22" s="143" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="137" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="114"/>
-      <c r="E23" s="143" t="s">
+      <c r="E23" s="137" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="114"/>
+      <c r="G23" s="143" t="s">
         <v>729</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="144" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="115"/>
-      <c r="E24" s="143" t="s">
+      <c r="E24" s="139" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="114"/>
+      <c r="G24" s="143" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="144" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="115"/>
-      <c r="E25" s="144" t="s">
+      <c r="E25" s="139" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="114"/>
+      <c r="G25" s="144" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="144" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="115"/>
-      <c r="E26" s="144" t="s">
+      <c r="E26" s="137" t="s">
+        <v>703</v>
+      </c>
+      <c r="F26" s="114"/>
+      <c r="G26" s="144" t="s">
         <v>731</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="144" t="s">
         <v>15</v>
       </c>
       <c r="C27" s="115"/>
-      <c r="E27" s="143" t="s">
+      <c r="E27" s="137" t="s">
+        <v>704</v>
+      </c>
+      <c r="F27" s="114"/>
+      <c r="G27" s="143" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" s="139" t="s">
         <v>16</v>
       </c>
       <c r="C28" s="114"/>
-      <c r="E28" s="137" t="s">
+      <c r="E28" s="139" t="s">
+        <v>705</v>
+      </c>
+      <c r="F28" s="114"/>
+      <c r="G28" s="137" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" s="139" t="s">
         <v>17</v>
       </c>
       <c r="C29" s="114"/>
-      <c r="E29" s="135" t="s">
+      <c r="E29" s="139" t="s">
+        <v>706</v>
+      </c>
+      <c r="F29" s="114"/>
+      <c r="G29" s="135" t="s">
         <v>1133</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B30" s="139" t="s">
         <v>688</v>
       </c>
       <c r="C30" s="114"/>
-      <c r="E30" s="145" t="s">
+      <c r="E30" s="137" t="s">
+        <v>707</v>
+      </c>
+      <c r="F30" s="114"/>
+      <c r="G30" s="145" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B31" s="144" t="s">
         <v>689</v>
       </c>
       <c r="C31" s="115"/>
-      <c r="E31" s="143" t="s">
+      <c r="E31" s="137" t="s">
+        <v>708</v>
+      </c>
+      <c r="F31" s="114"/>
+      <c r="G31" s="143" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B32" s="146" t="s">
         <v>690</v>
       </c>
       <c r="C32" s="115"/>
-      <c r="E32" s="146" t="s">
+      <c r="E32" s="137" t="s">
+        <v>709</v>
+      </c>
+      <c r="F32" s="114"/>
+      <c r="G32" s="146" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" s="146" t="s">
         <v>1138</v>
       </c>
       <c r="C33" s="115"/>
-      <c r="E33" s="146" t="s">
+      <c r="E33" s="137" t="s">
+        <v>710</v>
+      </c>
+      <c r="F33" s="114"/>
+      <c r="G33" s="146" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="144" t="s">
         <v>691</v>
       </c>
       <c r="C34" s="115"/>
-      <c r="E34" s="146" t="s">
+      <c r="E34" s="139" t="s">
+        <v>711</v>
+      </c>
+      <c r="F34" s="114"/>
+      <c r="G34" s="146" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="144" t="s">
         <v>692</v>
       </c>
       <c r="C35" s="115"/>
       <c r="E35" s="144" t="s">
+        <v>712</v>
+      </c>
+      <c r="F35" s="114"/>
+      <c r="G35" s="144" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B36" s="137" t="s">
         <v>693</v>
       </c>
       <c r="C36" s="114"/>
-      <c r="E36" s="144" t="s">
+      <c r="E36" s="146" t="s">
+        <v>713</v>
+      </c>
+      <c r="F36" s="114"/>
+      <c r="G36" s="144" t="s">
         <v>728</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B37" s="144" t="s">
         <v>18</v>
       </c>
       <c r="C37" s="115"/>
-      <c r="E37" s="138" t="s">
+      <c r="E37" s="146" t="s">
+        <v>714</v>
+      </c>
+      <c r="F37" s="114"/>
+      <c r="G37" s="138" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" s="144" t="s">
         <v>19</v>
       </c>
       <c r="C38" s="115"/>
-      <c r="E38" s="139" t="s">
+      <c r="E38" s="137" t="s">
+        <v>715</v>
+      </c>
+      <c r="F38" s="115"/>
+      <c r="G38" s="139" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" s="144" t="s">
         <v>20</v>
       </c>
       <c r="C39" s="115"/>
-      <c r="E39" s="143" t="s">
+      <c r="E39" s="140" t="s">
+        <v>716</v>
+      </c>
+      <c r="F39" s="115"/>
+      <c r="G39" s="143" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B40" s="144" t="s">
         <v>21</v>
       </c>
       <c r="C40" s="115"/>
-      <c r="E40" s="143" t="s">
+      <c r="E40" s="114"/>
+      <c r="F40" s="115"/>
+      <c r="G40" s="143" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B41" s="144" t="s">
         <v>22</v>
       </c>
       <c r="C41" s="115"/>
-      <c r="E41" s="143" t="s">
+      <c r="E41" s="141" t="s">
+        <v>1596</v>
+      </c>
+      <c r="F41" s="114"/>
+      <c r="G41" s="143" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B42" s="144" t="s">
         <v>23</v>
       </c>
       <c r="C42" s="115"/>
       <c r="E42" s="143" t="s">
+        <v>94</v>
+      </c>
+      <c r="F42" s="114"/>
+      <c r="G42" s="143" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B43" s="144" t="s">
         <v>24</v>
       </c>
       <c r="C43" s="115"/>
-      <c r="E43" s="143" t="s">
+      <c r="E43" s="147" t="s">
+        <v>95</v>
+      </c>
+      <c r="F43" s="114"/>
+      <c r="G43" s="143" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B44" s="144" t="s">
         <v>694</v>
       </c>
       <c r="C44" s="115"/>
       <c r="E44" s="147" t="s">
+        <v>96</v>
+      </c>
+      <c r="F44" s="117"/>
+      <c r="G44" s="147" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B45" s="144" t="s">
         <v>695</v>
       </c>
       <c r="C45" s="115"/>
-      <c r="E45" s="138" t="s">
+      <c r="E45" s="147" t="s">
+        <v>97</v>
+      </c>
+      <c r="F45" s="118"/>
+      <c r="G45" s="138" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B46" s="152" t="s">
         <v>889</v>
       </c>
       <c r="C46" s="116"/>
-      <c r="E46" s="137" t="s">
+      <c r="E46" s="147" t="s">
+        <v>98</v>
+      </c>
+      <c r="F46" s="118"/>
+      <c r="G46" s="137" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B47" s="144" t="s">
         <v>890</v>
       </c>
       <c r="C47" s="115"/>
-      <c r="E47" s="137" t="s">
+      <c r="E47" s="150" t="s">
+        <v>99</v>
+      </c>
+      <c r="F47" s="118"/>
+      <c r="G47" s="137" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B48" s="144" t="s">
         <v>891</v>
       </c>
       <c r="C48" s="115"/>
-      <c r="E48" s="137" t="s">
+      <c r="F48" s="118"/>
+      <c r="G48" s="137" t="s">
         <v>733</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" s="144" t="s">
         <v>893</v>
       </c>
       <c r="C49" s="115"/>
-      <c r="E49" s="137" t="s">
+      <c r="F49" s="118"/>
+      <c r="G49" s="137" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50" s="144" t="s">
         <v>894</v>
       </c>
       <c r="C50" s="115"/>
-      <c r="E50" s="137" t="s">
+      <c r="E50" s="115"/>
+      <c r="F50" s="114"/>
+      <c r="G50" s="137" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B51" s="137" t="s">
         <v>879</v>
       </c>
       <c r="C51" s="114"/>
-      <c r="E51" s="137" t="s">
+      <c r="G51" s="137" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B52" s="144" t="s">
         <v>25</v>
       </c>
       <c r="C52" s="115"/>
-      <c r="E52" s="137" t="s">
+      <c r="G52" s="137" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B53" s="144" t="s">
         <v>26</v>
       </c>
       <c r="C53" s="115"/>
-      <c r="E53" s="138" t="s">
+      <c r="D53" s="115"/>
+      <c r="E53" s="115"/>
+      <c r="G53" s="138" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B54" s="144" t="s">
         <v>27</v>
       </c>
       <c r="C54" s="115"/>
-      <c r="E54" s="139" t="s">
+      <c r="D54" s="115"/>
+      <c r="E54" s="115"/>
+      <c r="G54" s="139" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B55" s="144" t="s">
         <v>696</v>
       </c>
       <c r="C55" s="115"/>
-      <c r="E55" s="137" t="s">
+      <c r="D55" s="115"/>
+      <c r="E55" s="114"/>
+      <c r="G55" s="137" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B56" s="137" t="s">
         <v>880</v>
       </c>
       <c r="C56" s="114"/>
-      <c r="E56" s="139" t="s">
+      <c r="D56" s="114"/>
+      <c r="E56" s="117"/>
+      <c r="G56" s="139" t="s">
         <v>1547</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B57" s="135" t="s">
         <v>28</v>
       </c>
       <c r="C57" s="117"/>
-      <c r="E57" s="135" t="s">
+      <c r="D57" s="117"/>
+      <c r="E57" s="114"/>
+      <c r="G57" s="135" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B58" s="137" t="s">
         <v>29</v>
       </c>
       <c r="C58" s="114"/>
-      <c r="E58" s="137" t="s">
+      <c r="D58" s="114"/>
+      <c r="E58" s="114"/>
+      <c r="G58" s="137" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B59" s="137" t="s">
         <v>30</v>
       </c>
       <c r="C59" s="114"/>
-      <c r="E59" s="143" t="s">
+      <c r="D59" s="114"/>
+      <c r="E59" s="114"/>
+      <c r="G59" s="143" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B60" s="137" t="s">
         <v>31</v>
       </c>
       <c r="C60" s="114"/>
-      <c r="E60" s="143" t="s">
+      <c r="D60" s="114"/>
+      <c r="E60" s="117"/>
+      <c r="G60" s="143" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B61" s="135" t="s">
         <v>32</v>
       </c>
       <c r="C61" s="117"/>
-      <c r="E61" s="143" t="s">
+      <c r="D61" s="117"/>
+      <c r="E61" s="114"/>
+      <c r="G61" s="143" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B62" s="137" t="s">
         <v>33</v>
       </c>
       <c r="C62" s="114"/>
-      <c r="E62" s="143" t="s">
+      <c r="D62" s="114"/>
+      <c r="E62" s="114"/>
+      <c r="G62" s="143" t="s">
         <v>735</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B63" s="137" t="s">
         <v>34</v>
       </c>
       <c r="C63" s="114"/>
-      <c r="E63" s="143" t="s">
+      <c r="D63" s="114"/>
+      <c r="E63" s="114"/>
+      <c r="G63" s="143" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B64" s="137" t="s">
         <v>35</v>
       </c>
       <c r="C64" s="114"/>
-      <c r="E64" s="143" t="s">
+      <c r="D64" s="114"/>
+      <c r="G64" s="143" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B65" s="137" t="s">
         <v>36</v>
       </c>
       <c r="C65" s="114"/>
-      <c r="E65" s="143" t="s">
+      <c r="D65" s="114"/>
+      <c r="E65" s="114"/>
+      <c r="G65" s="143" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B66" s="137" t="s">
         <v>37</v>
       </c>
       <c r="C66" s="114"/>
-      <c r="E66" s="143" t="s">
+      <c r="D66" s="114"/>
+      <c r="E66" s="114"/>
+      <c r="G66" s="143" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B67" s="137" t="s">
         <v>38</v>
       </c>
       <c r="C67" s="114"/>
-      <c r="E67" s="138" t="s">
+      <c r="D67" s="114"/>
+      <c r="E67" s="114"/>
+      <c r="G67" s="138" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B68" s="135" t="s">
         <v>39</v>
       </c>
       <c r="C68" s="117"/>
-      <c r="E68" s="147" t="s">
+      <c r="D68" s="117"/>
+      <c r="E68" s="117"/>
+      <c r="G68" s="147" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B69" s="137" t="s">
         <v>40</v>
       </c>
       <c r="C69" s="114"/>
-      <c r="E69" s="144" t="s">
+      <c r="D69" s="114"/>
+      <c r="E69" s="114"/>
+      <c r="G69" s="144" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B70" s="137" t="s">
         <v>41</v>
       </c>
       <c r="C70" s="114"/>
-      <c r="E70" s="144" t="s">
+      <c r="D70" s="114"/>
+      <c r="E70" s="114"/>
+      <c r="G70" s="144" t="s">
         <v>740</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B71" s="137" t="s">
         <v>42</v>
       </c>
       <c r="C71" s="114"/>
-      <c r="E71" s="144" t="s">
+      <c r="D71" s="114"/>
+      <c r="E71" s="114"/>
+      <c r="G71" s="144" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B72" s="137" t="s">
         <v>43</v>
       </c>
       <c r="C72" s="114"/>
-      <c r="E72" s="143" t="s">
+      <c r="D72" s="114"/>
+      <c r="E72" s="114"/>
+      <c r="G72" s="143" t="s">
         <v>742</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B73" s="138" t="s">
         <v>44</v>
       </c>
       <c r="C73" s="117"/>
-      <c r="E73" s="143" t="s">
+      <c r="D73" s="117"/>
+      <c r="E73" s="117"/>
+      <c r="G73" s="143" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B74" s="137" t="s">
         <v>45</v>
       </c>
       <c r="C74" s="114"/>
-      <c r="E74" s="143" t="s">
+      <c r="D74" s="114"/>
+      <c r="E74" s="114"/>
+      <c r="G74" s="143" t="s">
         <v>743</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B75" s="137" t="s">
         <v>46</v>
       </c>
       <c r="C75" s="114"/>
-      <c r="E75" s="143" t="s">
+      <c r="D75" s="114"/>
+      <c r="E75" s="114"/>
+      <c r="G75" s="143" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B76" s="137" t="s">
         <v>47</v>
       </c>
       <c r="C76" s="114"/>
-      <c r="E76" s="143" t="s">
+      <c r="D76" s="114"/>
+      <c r="E76" s="127"/>
+      <c r="G76" s="143" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B77" s="137" t="s">
         <v>48</v>
       </c>
       <c r="C77" s="114"/>
-      <c r="E77" s="138" t="s">
+      <c r="D77" s="114"/>
+      <c r="E77" s="117"/>
+      <c r="G77" s="138" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B78" s="140" t="s">
         <v>697</v>
       </c>
       <c r="C78" s="114"/>
-      <c r="E78" s="138" t="s">
+      <c r="D78" s="114"/>
+      <c r="E78" s="134" t="s">
+        <v>1597</v>
+      </c>
+      <c r="G78" s="138" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B79" s="114"/>
       <c r="C79" s="114"/>
-      <c r="E79" s="143" t="s">
+      <c r="D79" s="114"/>
+      <c r="E79" s="135" t="s">
+        <v>133</v>
+      </c>
+      <c r="G79" s="143" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B80" s="127" t="s">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D80" s="127"/>
+      <c r="E80" s="136" t="s">
+        <v>134</v>
+      </c>
+      <c r="G80" s="143" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B81" s="127" t="s">
         <v>50</v>
       </c>
-      <c r="C80" s="127"/>
-      <c r="E80" s="143" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B81" s="141" t="s">
-        <v>1592</v>
-      </c>
-      <c r="C81" s="117"/>
-      <c r="E81" s="143" t="s">
+      <c r="D81" s="117"/>
+      <c r="E81" s="137" t="s">
+        <v>135</v>
+      </c>
+      <c r="G81" s="143" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B82" s="147" t="s">
-        <v>52</v>
-      </c>
-      <c r="C82" s="118"/>
-      <c r="E82" s="143" t="s">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D82" s="118"/>
+      <c r="E82" s="136" t="s">
+        <v>136</v>
+      </c>
+      <c r="G82" s="143" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B83" s="144" t="s">
-        <v>698</v>
-      </c>
-      <c r="C83" s="115"/>
-      <c r="E83" s="143" t="s">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D83" s="115"/>
+      <c r="E83" s="137" t="s">
+        <v>137</v>
+      </c>
+      <c r="G83" s="143" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B84" s="144" t="s">
-        <v>699</v>
-      </c>
-      <c r="C84" s="115"/>
-      <c r="E84" s="135" t="s">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D84" s="115"/>
+      <c r="E84" s="137" t="s">
+        <v>745</v>
+      </c>
+      <c r="G84" s="135" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B85" s="144" t="s">
-        <v>700</v>
-      </c>
-      <c r="C85" s="115"/>
-      <c r="E85" s="143" t="s">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D85" s="115"/>
+      <c r="E85" s="137" t="s">
+        <v>746</v>
+      </c>
+      <c r="G85" s="143" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B86" s="147" t="s">
-        <v>53</v>
-      </c>
-      <c r="C86" s="118"/>
-      <c r="E86" s="143" t="s">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D86" s="118"/>
+      <c r="E86" s="137" t="s">
+        <v>747</v>
+      </c>
+      <c r="G86" s="143" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B87" s="147" t="s">
-        <v>54</v>
-      </c>
-      <c r="C87" s="118"/>
-      <c r="E87" s="143" t="s">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D87" s="118"/>
+      <c r="E87" s="136" t="s">
+        <v>748</v>
+      </c>
+      <c r="G87" s="143" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B88" s="147" t="s">
-        <v>55</v>
-      </c>
-      <c r="C88" s="118"/>
-      <c r="E88" s="143" t="s">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D88" s="118"/>
+      <c r="E88" s="138" t="s">
+        <v>139</v>
+      </c>
+      <c r="G88" s="143" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B89" s="147" t="s">
-        <v>56</v>
-      </c>
-      <c r="C89" s="118"/>
-      <c r="E89" s="143" t="s">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D89" s="118"/>
+      <c r="E89" s="139" t="s">
+        <v>140</v>
+      </c>
+      <c r="G89" s="143" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B90" s="147" t="s">
-        <v>57</v>
-      </c>
-      <c r="C90" s="118"/>
-      <c r="E90" s="143" t="s">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D90" s="118"/>
+      <c r="E90" s="139" t="s">
+        <v>141</v>
+      </c>
+      <c r="G90" s="143" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B91" s="147" t="s">
-        <v>58</v>
-      </c>
-      <c r="C91" s="118"/>
-      <c r="E91" s="148" t="s">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D91" s="118"/>
+      <c r="E91" s="140" t="s">
+        <v>142</v>
+      </c>
+      <c r="G91" s="148" t="s">
         <v>1581</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B92" s="147" t="s">
-        <v>59</v>
-      </c>
-      <c r="C92" s="118"/>
-      <c r="E92" s="138" t="s">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D92" s="118"/>
+      <c r="G92" s="138" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B93" s="144" t="s">
-        <v>701</v>
-      </c>
-      <c r="C93" s="115"/>
-      <c r="E93" s="143" t="s">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D93" s="115"/>
+      <c r="E93" s="114"/>
+      <c r="G93" s="143" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B94" s="144" t="s">
-        <v>702</v>
-      </c>
-      <c r="C94" s="115"/>
-      <c r="E94" s="143" t="s">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D94" s="115"/>
+      <c r="G94" s="143" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B95" s="139" t="s">
-        <v>60</v>
-      </c>
-      <c r="C95" s="114"/>
-      <c r="E95" s="143" t="s">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D95" s="114"/>
+      <c r="G95" s="143" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B96" s="139" t="s">
-        <v>1373</v>
-      </c>
-      <c r="C96" s="114"/>
-      <c r="E96" s="149" t="s">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D96" s="114"/>
+      <c r="G96" s="149" t="s">
         <v>744</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B97" s="137" t="s">
-        <v>61</v>
-      </c>
-      <c r="C97" s="114"/>
-      <c r="E97" s="118"/>
-    </row>
-    <row r="98" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B98" s="137" t="s">
-        <v>62</v>
-      </c>
-      <c r="C98" s="114"/>
-      <c r="E98" s="134" t="s">
-        <v>1597</v>
-      </c>
-    </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B99" s="139" t="s">
-        <v>63</v>
-      </c>
-      <c r="C99" s="114"/>
-      <c r="E99" s="135" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B100" s="139" t="s">
-        <v>64</v>
-      </c>
-      <c r="C100" s="114"/>
-      <c r="E100" s="136" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B101" s="137" t="s">
-        <v>703</v>
-      </c>
-      <c r="C101" s="114"/>
-      <c r="E101" s="137" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B102" s="137" t="s">
-        <v>704</v>
-      </c>
-      <c r="C102" s="114"/>
-      <c r="E102" s="136" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B103" s="139" t="s">
-        <v>705</v>
-      </c>
-      <c r="C103" s="114"/>
-      <c r="E103" s="137" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B104" s="139" t="s">
-        <v>706</v>
-      </c>
-      <c r="C104" s="114"/>
-      <c r="E104" s="137" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B105" s="137" t="s">
-        <v>707</v>
-      </c>
-      <c r="C105" s="114"/>
-      <c r="E105" s="137" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B106" s="137" t="s">
-        <v>708</v>
-      </c>
-      <c r="C106" s="114"/>
-      <c r="E106" s="137" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B107" s="137" t="s">
-        <v>709</v>
-      </c>
-      <c r="C107" s="114"/>
-      <c r="E107" s="136" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B108" s="137" t="s">
-        <v>710</v>
-      </c>
-      <c r="C108" s="114"/>
-      <c r="E108" s="138" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B109" s="139" t="s">
-        <v>711</v>
-      </c>
-      <c r="C109" s="114"/>
-      <c r="E109" s="139" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B110" s="144" t="s">
-        <v>712</v>
-      </c>
-      <c r="C110" s="115"/>
-      <c r="E110" s="139" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B111" s="146" t="s">
-        <v>713</v>
-      </c>
-      <c r="C111" s="115"/>
-      <c r="D111" s="126"/>
-      <c r="E111" s="140" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B112" s="146" t="s">
-        <v>714</v>
-      </c>
-      <c r="C112" s="115"/>
-      <c r="D112" s="126"/>
-    </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B113" s="137" t="s">
-        <v>715</v>
-      </c>
-      <c r="C113" s="114"/>
-      <c r="D113" s="126"/>
-    </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B114" s="140" t="s">
-        <v>716</v>
-      </c>
-      <c r="C114" s="114"/>
-      <c r="D114" s="126"/>
-    </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B115" s="114"/>
-      <c r="C115" s="114"/>
-    </row>
-    <row r="116" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B116" s="141" t="s">
-        <v>1596</v>
-      </c>
-      <c r="C116" s="117"/>
-    </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B117" s="143" t="s">
-        <v>94</v>
-      </c>
-      <c r="C117" s="118"/>
-    </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B118" s="147" t="s">
-        <v>95</v>
-      </c>
-      <c r="C118" s="118"/>
-    </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B119" s="147" t="s">
-        <v>96</v>
-      </c>
-      <c r="C119" s="118"/>
-      <c r="E119" s="124" t="s">
+    <row r="97" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D97" s="114"/>
+      <c r="G97" s="118"/>
+    </row>
+    <row r="98" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D98" s="114"/>
+      <c r="E98" s="114"/>
+    </row>
+    <row r="99" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D99" s="114"/>
+      <c r="E99" s="114"/>
+    </row>
+    <row r="100" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D100" s="114"/>
+      <c r="E100" s="114"/>
+    </row>
+    <row r="101" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D101" s="114"/>
+      <c r="E101" s="114"/>
+    </row>
+    <row r="102" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D102" s="114"/>
+      <c r="E102" s="114"/>
+    </row>
+    <row r="103" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D103" s="114"/>
+      <c r="E103" s="114"/>
+    </row>
+    <row r="104" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D104" s="114"/>
+      <c r="E104" s="114"/>
+    </row>
+    <row r="105" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D105" s="114"/>
+      <c r="E105" s="114"/>
+    </row>
+    <row r="106" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D106" s="114"/>
+      <c r="E106" s="114"/>
+    </row>
+    <row r="107" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D107" s="114"/>
+      <c r="E107" s="114"/>
+    </row>
+    <row r="108" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D108" s="114"/>
+      <c r="E108" s="114"/>
+    </row>
+    <row r="109" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D109" s="114"/>
+      <c r="E109" s="114"/>
+    </row>
+    <row r="110" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D110" s="115"/>
+      <c r="E110" s="115"/>
+    </row>
+    <row r="111" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D111" s="115"/>
+      <c r="E111" s="115"/>
+      <c r="F111" s="126"/>
+    </row>
+    <row r="112" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D112" s="115"/>
+      <c r="E112" s="115"/>
+      <c r="F112" s="126"/>
+    </row>
+    <row r="113" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D113" s="114"/>
+      <c r="E113" s="114"/>
+      <c r="F113" s="126"/>
+    </row>
+    <row r="114" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D114" s="114"/>
+      <c r="E114" s="114"/>
+      <c r="F114" s="126"/>
+    </row>
+    <row r="115" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D115" s="114"/>
+      <c r="E115" s="114"/>
+    </row>
+    <row r="116" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D116" s="117"/>
+      <c r="E116" s="117"/>
+    </row>
+    <row r="117" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D117" s="118"/>
+      <c r="E117" s="118"/>
+    </row>
+    <row r="118" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D118" s="118"/>
+      <c r="E118" s="118"/>
+    </row>
+    <row r="119" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D119" s="118"/>
+      <c r="E119" s="118"/>
+      <c r="G119" s="124" t="s">
         <v>952</v>
       </c>
     </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B120" s="147" t="s">
-        <v>97</v>
-      </c>
-      <c r="C120" s="118"/>
-    </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B121" s="147" t="s">
-        <v>98</v>
-      </c>
-      <c r="C121" s="118"/>
-    </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B122" s="150" t="s">
-        <v>99</v>
-      </c>
-      <c r="C122" s="114"/>
+    <row r="120" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D120" s="118"/>
+      <c r="E120" s="118"/>
+    </row>
+    <row r="121" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D121" s="118"/>
+      <c r="E121" s="118"/>
+    </row>
+    <row r="122" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D122" s="114"/>
+      <c r="E122" s="114"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>